<commit_message>
Included missing group in DIF analyses for migration in data example 1.
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/ex1/tables/dif_dich_TR.xlsx
+++ b/tests/testthat/fixtures/ex1/tables/dif_dich_TR.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t xml:space="preserve">DIF.variable</t>
   </si>
@@ -54,7 +54,13 @@
     <t xml:space="preserve">sex 0-1</t>
   </si>
   <si>
-    <t xml:space="preserve">mig 0-1</t>
+    <t xml:space="preserve">mig 1-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mig 1-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mig 2-3</t>
   </si>
   <si>
     <t xml:space="preserve">grk10001_c</t>
@@ -63,7 +69,13 @@
     <t xml:space="preserve">-0.007 (-0.006)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.016 ( 0.014)</t>
+    <t xml:space="preserve"> 0.017 ( 0.015)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.519 (-0.444)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.536 (-0.459)</t>
   </si>
   <si>
     <t xml:space="preserve">grk10002_c</t>
@@ -75,13 +87,25 @@
     <t xml:space="preserve">-0.023 (-0.020)</t>
   </si>
   <si>
+    <t xml:space="preserve"> 0.226 ( 0.193)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.250 ( 0.214)</t>
+  </si>
+  <si>
     <t xml:space="preserve">grk10003_c</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.062 ( 0.052)</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.064 (-0.056)</t>
+    <t xml:space="preserve">-0.064 (-0.055)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.137 (-0.117)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.073 (-0.062)</t>
   </si>
   <si>
     <t xml:space="preserve">grk10004_c</t>
@@ -90,7 +114,13 @@
     <t xml:space="preserve"> 0.109 ( 0.091)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.252 ( 0.222)</t>
+    <t xml:space="preserve"> 0.253 ( 0.217)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.244 ( 0.209)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.009 (-0.008)</t>
   </si>
   <si>
     <t xml:space="preserve">grk10005_c</t>
@@ -99,7 +129,13 @@
     <t xml:space="preserve">-0.126 (-0.106)</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.257 (-0.227)</t>
+    <t xml:space="preserve">-0.259 (-0.222)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.345 ( 0.295)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.603 ( 0.516)</t>
   </si>
   <si>
     <t xml:space="preserve">grk10006_c</t>
@@ -108,7 +144,13 @@
     <t xml:space="preserve"> 0.011 ( 0.009)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.094 ( 0.083)</t>
+    <t xml:space="preserve"> 0.094 ( 0.080)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.359 ( 0.307)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.265 ( 0.227)</t>
   </si>
   <si>
     <t xml:space="preserve">grk10007_c</t>
@@ -117,7 +159,13 @@
     <t xml:space="preserve">-0.031 (-0.026)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.077 ( 0.068)</t>
+    <t xml:space="preserve"> 0.078 ( 0.067)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.164 ( 0.140)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.086 ( 0.074)</t>
   </si>
   <si>
     <t xml:space="preserve">grk10008_c</t>
@@ -126,7 +174,13 @@
     <t xml:space="preserve">-0.077 (-0.064)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.095 ( 0.084)</t>
+    <t xml:space="preserve"> 0.096 ( 0.082)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.026 (-0.022)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.122 (-0.104)</t>
   </si>
   <si>
     <t xml:space="preserve">grk10009_c</t>
@@ -135,7 +189,13 @@
     <t xml:space="preserve">-0.024 (-0.020)</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.071 (-0.063)</t>
+    <t xml:space="preserve">-0.071 (-0.061)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.110 ( 0.094)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.181 ( 0.155)</t>
   </si>
   <si>
     <t xml:space="preserve">grk10010_c</t>
@@ -144,7 +204,13 @@
     <t xml:space="preserve">-0.066 (-0.055)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.054 ( 0.048)</t>
+    <t xml:space="preserve"> 0.054 ( 0.046)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.112 (-0.096)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.166 (-0.142)</t>
   </si>
   <si>
     <t xml:space="preserve">grk10011_c</t>
@@ -153,7 +219,7 @@
     <t xml:space="preserve">-0.019 (-0.016)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.179 ( 0.158)</t>
+    <t xml:space="preserve">-0.199 (-0.170)</t>
   </si>
   <si>
     <t xml:space="preserve">grk10012_c</t>
@@ -162,7 +228,13 @@
     <t xml:space="preserve">-0.296 (-0.248)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.140 ( 0.124)</t>
+    <t xml:space="preserve"> 0.141 ( 0.121)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.094 (-0.080)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.235 (-0.201)</t>
   </si>
   <si>
     <t xml:space="preserve">grk10013_c</t>
@@ -171,7 +243,13 @@
     <t xml:space="preserve"> 0.147 ( 0.123)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.091 ( 0.080)</t>
+    <t xml:space="preserve"> 0.090 ( 0.077)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.115 (-0.098)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.205 (-0.175)</t>
   </si>
   <si>
     <t xml:space="preserve">grk10014_c</t>
@@ -180,7 +258,13 @@
     <t xml:space="preserve"> 0.153 ( 0.128)</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.130 (-0.115)</t>
+    <t xml:space="preserve">-0.131 (-0.112)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.026 ( 0.022)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.157 ( 0.134)</t>
   </si>
   <si>
     <t xml:space="preserve">grk10015_c</t>
@@ -189,7 +273,13 @@
     <t xml:space="preserve">-0.220 (-0.184)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.453 ( 0.400)</t>
+    <t xml:space="preserve"> 0.456 ( 0.390)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.452 ( 0.387)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.004 (-0.003)</t>
   </si>
   <si>
     <t xml:space="preserve">Main effect (DIF model)</t>
@@ -198,7 +288,13 @@
     <t xml:space="preserve">-0.422 (-0.354)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.750 (0.662)</t>
+    <t xml:space="preserve">0.756 (0.647)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.538 (0.461)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.218 (-0.187)</t>
   </si>
   <si>
     <t xml:space="preserve">Main effect (Main effect model)</t>
@@ -207,7 +303,13 @@
     <t xml:space="preserve">-0.401 (-0.336)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.724 (0.640)</t>
+    <t xml:space="preserve">0.730 (0.627)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.497 (0.427)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.233 (-0.200)</t>
   </si>
 </sst>
 </file>
@@ -616,19 +718,19 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>814</v>
+        <v>1000</v>
       </c>
       <c r="D4" t="n">
-        <v>11041</v>
+        <v>13597</v>
       </c>
       <c r="E4" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" t="n">
-        <v>11075</v>
+        <v>13633</v>
       </c>
       <c r="G4" t="n">
-        <v>11155</v>
+        <v>13721</v>
       </c>
     </row>
     <row r="5">
@@ -639,19 +741,19 @@
         <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>814</v>
+        <v>1000</v>
       </c>
       <c r="D5" t="n">
-        <v>11032</v>
+        <v>13570</v>
       </c>
       <c r="E5" t="n">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="F5" t="n">
-        <v>11094</v>
+        <v>13662</v>
       </c>
       <c r="G5" t="n">
-        <v>11240</v>
+        <v>13888</v>
       </c>
     </row>
   </sheetData>
@@ -678,192 +780,300 @@
       <c r="C1" t="s">
         <v>13</v>
       </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>60</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>76</v>
+      </c>
+      <c r="D14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>81</v>
+      </c>
+      <c r="D15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>86</v>
+      </c>
+      <c r="D16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>91</v>
+      </c>
+      <c r="D17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>96</v>
+      </c>
+      <c r="D18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>